<commit_message>
add new collaborator testing
</commit_message>
<xml_diff>
--- a/Phase 3/ST-COMM-Testing-phase3/cancelGame.xlsx
+++ b/Phase 3/ST-COMM-Testing-phase3/cancelGame.xlsx
@@ -39,10 +39,10 @@
     <t>Add</t>
   </si>
   <si>
-    <t>Keven</t>
-  </si>
-  <si>
     <t>123X456</t>
+  </si>
+  <si>
+    <t>andrew</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -388,10 +388,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>

</xml_diff>